<commit_message>
updated import files to match improvements in tests
git-svn-id: https://svn.fao.org/projects/ruralinvest/RIV4/trunk@66878 d7fa552c-c32d-11e1-9f2d-6d39f2a56844
</commit_message>
<xml_diff>
--- a/RIV4-tests/src/test/resources/imports/project/project-invest-nig.xlsx
+++ b/RIV4-tests/src/test/resources/imports/project/project-invest-nig.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="41">
   <si>
     <t>Investment detail</t>
   </si>
@@ -139,6 +139,10 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Very Minor Works</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -530,14 +534,15 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:XFD24"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" customWidth="1"/>
     <col min="4" max="8" width="8.83203125" style="4"/>
     <col min="10" max="11" width="8.83203125" style="4"/>
@@ -951,119 +956,119 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="D15" s="1" t="s">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>1450</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <f>C15*D15</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>0</v>
+      </c>
+      <c r="H15" s="4">
+        <f>E15-F15-G15</f>
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="D16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E16" s="4">
         <f>SUM(E14:E14)</f>
         <v>32625</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F16" s="4">
         <f>SUM(F14:F14)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G16" s="4">
         <f>SUM(G14:G14)</f>
         <v>13500</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H16" s="4">
         <f>SUM(H14:H14)</f>
         <v>19125</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="18">
-      <c r="A17" s="3" t="s">
+    <row r="18" spans="1:13" ht="18">
+      <c r="A18" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:13">
+      <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-      <c r="D19" s="4">
-        <v>250000</v>
-      </c>
-      <c r="E19" s="4">
-        <f>C19*D19</f>
-        <v>250000</v>
-      </c>
-      <c r="F19" s="4">
-        <v>0</v>
-      </c>
-      <c r="G19" s="4">
-        <v>0</v>
-      </c>
-      <c r="H19" s="4">
-        <f>E19-F19-G19</f>
-        <v>250000</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C20">
-        <v>60</v>
+        <v>1</v>
       </c>
       <c r="D20" s="4">
-        <v>3800</v>
+        <v>250000</v>
       </c>
       <c r="E20" s="4">
         <f>C20*D20</f>
-        <v>228000</v>
+        <v>250000</v>
       </c>
       <c r="F20" s="4">
         <v>0</v>
@@ -1073,7 +1078,7 @@
       </c>
       <c r="H20" s="4">
         <f>E20-F20-G20</f>
-        <v>228000</v>
+        <v>250000</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -1081,20 +1086,20 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="D21" s="4">
-        <v>7500</v>
+        <v>3800</v>
       </c>
       <c r="E21" s="4">
         <f>C21*D21</f>
-        <v>225000</v>
+        <v>228000</v>
       </c>
       <c r="F21" s="4">
         <v>0</v>
@@ -1104,7 +1109,7 @@
       </c>
       <c r="H21" s="4">
         <f>E21-F21-G21</f>
-        <v>225000</v>
+        <v>228000</v>
       </c>
       <c r="M21">
         <v>1</v>
@@ -1112,20 +1117,20 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B22" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C22">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="D22" s="4">
-        <v>1050000</v>
+        <v>7500</v>
       </c>
       <c r="E22" s="4">
         <f>C22*D22</f>
-        <v>1050000</v>
+        <v>225000</v>
       </c>
       <c r="F22" s="4">
         <v>0</v>
@@ -1135,62 +1140,92 @@
       </c>
       <c r="H22" s="4">
         <f>E22-F22-G22</f>
+        <v>225000</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" s="4">
         <v>1050000</v>
       </c>
-      <c r="M22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13">
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="4">
+        <f>C23*D23</f>
+        <v>1050000</v>
+      </c>
+      <c r="F23" s="4">
+        <v>0</v>
+      </c>
+      <c r="G23" s="4">
+        <v>0</v>
+      </c>
+      <c r="H23" s="4">
+        <f>E23-F23-G23</f>
+        <v>1050000</v>
+      </c>
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="D24" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E23" s="4">
-        <f>SUM(E19:E22)</f>
+      <c r="E24" s="4">
+        <f>SUM(E20:E23)</f>
         <v>1753000</v>
       </c>
-      <c r="F23" s="4">
-        <f>SUM(F19:F22)</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="4">
-        <f>SUM(G19:G22)</f>
-        <v>0</v>
-      </c>
-      <c r="H23" s="4">
-        <f>SUM(H19:H22)</f>
+      <c r="F24" s="4">
+        <f>SUM(F20:F23)</f>
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <f>SUM(G20:G23)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <f>SUM(H20:H23)</f>
         <v>1753000</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
-      <c r="D24" s="1"/>
-    </row>
     <row r="25" spans="1:13">
-      <c r="D25" s="1" t="s">
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:13">
+      <c r="D26" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="4">
-        <f>E10+E15+E23</f>
+      <c r="E26" s="4">
+        <f>E10+E16+E24</f>
         <v>9532625</v>
       </c>
-      <c r="F25" s="4">
-        <f>F10+F15+F23</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="4">
-        <f>G10+G15+G23</f>
+      <c r="F26" s="4">
+        <f>F10+F16+F24</f>
+        <v>0</v>
+      </c>
+      <c r="G26" s="4">
+        <f>G10+G16+G24</f>
         <v>1013500</v>
       </c>
-      <c r="H25" s="4">
-        <f>H10+H15+H23</f>
+      <c r="H26" s="4">
+        <f>H10+H16+H24</f>
         <v>8519125</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B14">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B14:B15">
       <formula1>"p/day(s),p/week(s),p/month(s),p/year(s)"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>